<commit_message>
MS: additional unit tests for getLastRow, appendNamedRegion & appendWorksheet
git-svn-id: svn://ms72.weblink.ch/mirai/XLConnect-R@139 ccc6e944-403e-a54a-b5f3-c2babcd103ea
</commit_message>
<xml_diff>
--- a/inst/unitTests/resources/testWorkbookGetLastRow.xlsx
+++ b/inst/unitTests/resources/testWorkbookGetLastRow.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="555" windowWidth="19815" windowHeight="7620"/>
+    <workbookView xWindow="750" yWindow="555" windowWidth="19815" windowHeight="7620" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="mtcars" sheetId="1" r:id="rId1"/>
     <sheet name="mtcars2" sheetId="2" r:id="rId2"/>
     <sheet name="mtcars3" sheetId="3" r:id="rId3"/>
+    <sheet name="empty" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="mtcars">mtcars!$A$1:$K$33</definedName>
@@ -402,7 +403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
@@ -3953,4 +3954,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>